<commit_message>
Commit the Lession2 change
</commit_message>
<xml_diff>
--- a/Documentation/02_Task/Lession2.xlsx
+++ b/Documentation/02_Task/Lession2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Write 1 demo on stm32f7, using task</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>8h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Testing message</t>
   </si>
 </sst>
 </file>
@@ -376,19 +379,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -402,12 +405,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -419,6 +422,14 @@
       </c>
       <c r="E3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>